<commit_message>
Butman_2007: Updated USDA soil type
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Butman_2007.xlsx
+++ b/ISRaD_data_files/Butman_2007.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfromm\Documents\GitHub\ISRaD\ISRaD_data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F1B630-595D-4E17-B2A7-0DC6336AE8AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="13580" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28716" windowHeight="13584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="901">
   <si>
     <t>entry_name</t>
   </si>
@@ -2690,12 +2696,54 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
+  </si>
+  <si>
+    <t>pro_usda_soil_order</t>
+  </si>
+  <si>
+    <t>Alfisols</t>
+  </si>
+  <si>
+    <t>Andisols</t>
+  </si>
+  <si>
+    <t>Aridisols</t>
+  </si>
+  <si>
+    <t>Entisols</t>
+  </si>
+  <si>
+    <t>Gelisols</t>
+  </si>
+  <si>
+    <t>Histosols</t>
+  </si>
+  <si>
+    <t>Inceptisols</t>
+  </si>
+  <si>
+    <t>Mollisols</t>
+  </si>
+  <si>
+    <t>Oxisols</t>
+  </si>
+  <si>
+    <t>Spodosols</t>
+  </si>
+  <si>
+    <t>Ultisols</t>
+  </si>
+  <si>
+    <t>Vertisols</t>
+  </si>
+  <si>
+    <t>Cheshire–Holyoke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2834,10 +2882,18 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_layer" xfId="3"/>
+    <cellStyle name="Normal_layer" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3119,14 +3175,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3176,7 +3234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3223,7 +3281,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3261,7 +3319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3314,16 +3372,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3346,7 +3404,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3369,7 +3427,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3386,7 +3444,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3415,19 +3473,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3468,76 +3526,79 @@
         <v>82</v>
       </c>
       <c r="N1" t="s">
+        <v>887</v>
+      </c>
+      <c r="O1" t="s">
         <v>83</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>84</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>86</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>87</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>88</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>89</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>90</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>91</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>94</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>97</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>98</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>99</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>100</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>101</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>102</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>103</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>104</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3577,77 +3638,77 @@
       <c r="M2" t="s">
         <v>114</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>115</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>116</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>117</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>118</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>119</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>120</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>121</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>122</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>123</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>124</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>125</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>126</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>127</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>128</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>129</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>130</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>131</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>132</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>133</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>134</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>135</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>136</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3675,29 +3736,26 @@
       <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>143</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>144</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>145</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>142</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>146</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>147</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>148</v>
-      </c>
-      <c r="V3" t="s">
-        <v>149</v>
       </c>
       <c r="W3" t="s">
         <v>149</v>
@@ -3706,43 +3764,46 @@
         <v>149</v>
       </c>
       <c r="Y3" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z3" t="s">
         <v>150</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>151</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>152</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>153</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>154</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>155</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>146</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>156</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>157</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>158</v>
       </c>
       <c r="AI3" t="s">
         <v>158</v>
       </c>
       <c r="AJ3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3755,10 +3816,19 @@
       <c r="H4" t="s">
         <v>159</v>
       </c>
-      <c r="T4" t="s">
+      <c r="N4" t="s">
+        <v>894</v>
+      </c>
+      <c r="P4" t="s">
+        <v>900</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>160</v>
+      </c>
+      <c r="U4" t="s">
         <v>161</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3774,14 +3844,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3894,7 +3964,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4004,7 +4074,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4096,16 +4166,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CT6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4401,7 +4471,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4697,7 +4767,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4936,7 +5006,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4971,7 +5041,7 @@
         <v>0.87599999999999989</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5006,7 +5076,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5053,14 +5123,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5146,7 +5216,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5229,7 +5299,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5288,16 +5358,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="52">
+    <row r="1" spans="1:73" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5518,7 +5588,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5736,7 +5806,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5915,14 +5985,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6014,7 +6084,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6097,7 +6167,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6156,14 +6226,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AS21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>638</v>
       </c>
@@ -6176,128 +6248,128 @@
       <c r="D1" t="s">
         <v>641</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>642</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>643</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>644</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>645</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>646</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>647</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>648</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>649</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>650</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>651</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>652</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>653</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>654</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>655</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>656</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>657</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>658</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>659</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>660</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>661</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>662</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>663</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>664</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>665</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>666</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>667</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>668</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>669</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>670</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>671</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>672</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>673</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>674</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>675</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>676</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>677</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>678</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>679</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>680</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -6311,150 +6383,153 @@
         <v>101</v>
       </c>
       <c r="E2" t="s">
+        <v>887</v>
+      </c>
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>89</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>102</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>94</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>97</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>77</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>168</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>170</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>171</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>172</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>174</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>176</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>177</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>178</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>184</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>261</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>266</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>295</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>245</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>249</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>252</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>682</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>454</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>455</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>456</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>457</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>463</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>593</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>683</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>599</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>601</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>603</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>606</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>496</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>500</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>495</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>497</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>502</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
-      <c r="G3" t="s">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
         <v>684</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>685</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>686</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>685</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>562</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>687</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>689</v>
       </c>
@@ -6468,127 +6543,130 @@
         <v>692</v>
       </c>
       <c r="E4" t="s">
+        <v>888</v>
+      </c>
+      <c r="F4" t="s">
         <v>160</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>693</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>694</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>695</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>696</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>697</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>159</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>698</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>699</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>700</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>701</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>702</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>703</v>
-      </c>
-      <c r="R4" t="s">
-        <v>691</v>
       </c>
       <c r="S4" t="s">
         <v>691</v>
       </c>
       <c r="T4" t="s">
+        <v>691</v>
+      </c>
+      <c r="U4" t="s">
         <v>704</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>705</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>706</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>707</v>
-      </c>
-      <c r="X4" t="s">
-        <v>691</v>
       </c>
       <c r="Y4" t="s">
         <v>691</v>
       </c>
       <c r="Z4" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA4" t="s">
         <v>708</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>709</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>710</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>699</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>711</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>702</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>712</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>713</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>700</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>714</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>715</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>716</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>717</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>718</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>719</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>720</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>721</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>691</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>722</v>
       </c>
@@ -6599,109 +6677,112 @@
         <v>724</v>
       </c>
       <c r="E5" t="s">
+        <v>889</v>
+      </c>
+      <c r="F5" t="s">
         <v>725</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>726</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>727</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>728</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>729</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>730</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>731</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>732</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>733</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>734</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>735</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>736</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>737</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>738</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>739</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>740</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>741</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>742</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>743</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>733</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>744</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>736</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>745</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>746</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>734</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>747</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>748</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>749</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>750</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>751</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>752</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>753</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>754</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>755</v>
       </c>
@@ -6712,447 +6793,477 @@
         <v>757</v>
       </c>
       <c r="E6" t="s">
+        <v>890</v>
+      </c>
+      <c r="F6" t="s">
         <v>758</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>161</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>759</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>760</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>761</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>762</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>763</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>764</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>765</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>766</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>767</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>492</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>768</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>769</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>770</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>771</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>772</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>773</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>764</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>767</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>774</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>775</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>776</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>777</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>758</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>778</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>779</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>780</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>36</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>781</v>
       </c>
       <c r="B7" t="s">
         <v>782</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
+        <v>891</v>
+      </c>
+      <c r="G7" t="s">
         <v>783</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>784</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>785</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>786</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>787</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>788</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>789</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>790</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>791</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>792</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>793</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>794</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>788</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>790</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>795</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>796</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>797</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>798</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>799</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>800</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>801</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>802</v>
       </c>
       <c r="B8" t="s">
         <v>803</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
+        <v>892</v>
+      </c>
+      <c r="G8" t="s">
         <v>804</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>805</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>806</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>807</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>808</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>809</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>810</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>811</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>812</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>813</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>814</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>758</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>809</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>811</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
         <v>815</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AN8" t="s">
         <v>816</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AO8" t="s">
         <v>817</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AP8" t="s">
         <v>818</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AQ8" t="s">
         <v>492</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AS8" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>819</v>
       </c>
       <c r="B9" t="s">
         <v>820</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>893</v>
+      </c>
+      <c r="G9" t="s">
         <v>821</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>822</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>823</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>824</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>825</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>826</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>827</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>828</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>829</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>830</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>826</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AN9" t="s">
         <v>831</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>832</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>833</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>835</v>
       </c>
       <c r="B10" t="s">
         <v>836</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
+        <v>894</v>
+      </c>
+      <c r="G10" t="s">
         <v>837</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>838</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>839</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>840</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AN10" t="s">
         <v>841</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
         <v>842</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>843</v>
       </c>
-      <c r="AP10" t="s">
+      <c r="AQ10" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>845</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
+        <v>895</v>
+      </c>
+      <c r="G11" t="s">
         <v>846</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>847</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>848</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AN11" t="s">
         <v>849</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>850</v>
       </c>
       <c r="AO11" t="s">
         <v>850</v>
       </c>
       <c r="AP11" t="s">
+        <v>850</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
-      <c r="H12" t="s">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>896</v>
+      </c>
+      <c r="I12" t="s">
         <v>852</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>853</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AN12" t="s">
         <v>854</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
         <v>855</v>
       </c>
-      <c r="AO12" t="s">
+      <c r="AP12" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
-      <c r="U13" t="s">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>897</v>
+      </c>
+      <c r="V13" t="s">
         <v>857</v>
       </c>
-      <c r="AM13" t="s">
+      <c r="AN13" t="s">
         <v>858</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AO13" t="s">
         <v>859</v>
       </c>
-      <c r="AO13" t="s">
+      <c r="AP13" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
-      <c r="U14" t="s">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>898</v>
+      </c>
+      <c r="V14" t="s">
         <v>861</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>862</v>
       </c>
-      <c r="AO14" t="s">
+      <c r="AP14" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
-      <c r="U15" t="s">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>899</v>
+      </c>
+      <c r="V15" t="s">
         <v>864</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
         <v>865</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AP15" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
-      <c r="U16" t="s">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="V16" t="s">
         <v>867</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AO16" t="s">
         <v>868</v>
       </c>
-      <c r="AO16" t="s">
+      <c r="AP16" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="17" spans="40:41">
-      <c r="AN17" t="s">
+    <row r="17" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO17" t="s">
         <v>870</v>
       </c>
-      <c r="AO17" t="s">
+      <c r="AP17" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="18" spans="40:41">
-      <c r="AN18" t="s">
+    <row r="18" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO18" t="s">
         <v>872</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AP18" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="19" spans="40:41">
-      <c r="AN19" t="s">
+    <row r="19" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO19" t="s">
         <v>874</v>
       </c>
-      <c r="AO19" t="s">
+      <c r="AP19" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="20" spans="40:41">
-      <c r="AN20" t="s">
+    <row r="20" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO20" t="s">
         <v>876</v>
       </c>
-      <c r="AO20" t="s">
+      <c r="AP20" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="21" spans="40:41">
-      <c r="AN21" t="s">
+    <row r="21" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO21" t="s">
         <v>878</v>
       </c>
     </row>

</xml_diff>